<commit_message>
build 8: crawler description product
</commit_message>
<xml_diff>
--- a/data/laptop_all.xlsx
+++ b/data/laptop_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\khanhpham\rag_chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA47858-EDA5-40BA-A5CF-574594AC235A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFF4C1D-D094-4AEA-9117-6122553BB22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3322,13 +3322,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA57ADB-4E89-4F84-A381-48570A685649}" name="Table2" displayName="Table2" ref="A1:Q332" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17">
-  <autoFilter ref="A1:Q332" xr:uid="{9DA57ADB-4E89-4F84-A381-48570A685649}">
-    <filterColumn colId="14">
-      <filters>
-        <filter val="Chromebook "/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q332" xr:uid="{9DA57ADB-4E89-4F84-A381-48570A685649}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q332">
     <sortCondition ref="K1:K332"/>
   </sortState>
@@ -3555,33 +3549,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="24" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="24" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3634,7 +3628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>919</v>
       </c>
@@ -3684,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>889</v>
       </c>
@@ -3737,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>944</v>
       </c>
@@ -3790,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>815</v>
       </c>
@@ -3840,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>813</v>
       </c>
@@ -3890,7 +3884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>817</v>
       </c>
@@ -3940,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>936</v>
       </c>
@@ -3993,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>783</v>
       </c>
@@ -4046,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>796</v>
       </c>
@@ -4099,7 +4093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>461</v>
       </c>
@@ -4152,7 +4146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>285</v>
       </c>
@@ -4205,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>348</v>
       </c>
@@ -4258,7 +4252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>299</v>
       </c>
@@ -4311,7 +4305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>306</v>
       </c>
@@ -4364,7 +4358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>565</v>
       </c>
@@ -4417,7 +4411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>658</v>
       </c>
@@ -4470,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>572</v>
       </c>
@@ -4523,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>478</v>
       </c>
@@ -4576,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>172</v>
       </c>
@@ -4629,7 +4623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>177</v>
       </c>
@@ -4682,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>181</v>
       </c>
@@ -4735,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>179</v>
       </c>
@@ -4788,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -4838,7 +4832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>206</v>
       </c>
@@ -4888,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>109</v>
       </c>
@@ -4941,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>125</v>
       </c>
@@ -4991,7 +4985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>139</v>
       </c>
@@ -5041,7 +5035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>100</v>
       </c>
@@ -5094,7 +5088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>631</v>
       </c>
@@ -5147,7 +5141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>157</v>
       </c>
@@ -5200,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>372</v>
       </c>
@@ -5250,7 +5244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>273</v>
       </c>
@@ -5303,7 +5297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>370</v>
       </c>
@@ -5353,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>116</v>
       </c>
@@ -5406,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -5459,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>374</v>
       </c>
@@ -5509,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>143</v>
       </c>
@@ -5562,7 +5556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>148</v>
       </c>
@@ -5615,7 +5609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>640</v>
       </c>
@@ -5668,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>644</v>
       </c>
@@ -5718,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>504</v>
       </c>
@@ -5771,7 +5765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>533</v>
       </c>
@@ -5824,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>729</v>
       </c>
@@ -5877,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>739</v>
       </c>
@@ -5930,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>765</v>
       </c>
@@ -5980,7 +5974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>807</v>
       </c>
@@ -6030,7 +6024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>558</v>
       </c>
@@ -6083,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>610</v>
       </c>
@@ -6136,7 +6130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>585</v>
       </c>
@@ -6189,7 +6183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>674</v>
       </c>
@@ -6239,7 +6233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>551</v>
       </c>
@@ -6292,7 +6286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>628</v>
       </c>
@@ -6345,7 +6339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>254</v>
       </c>
@@ -6398,7 +6392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>613</v>
       </c>
@@ -6451,7 +6445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>680</v>
       </c>
@@ -6501,7 +6495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>726</v>
       </c>
@@ -6554,7 +6548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>670</v>
       </c>
@@ -6604,7 +6598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>677</v>
       </c>
@@ -6654,7 +6648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>237</v>
       </c>
@@ -6707,7 +6701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>542</v>
       </c>
@@ -6760,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>325</v>
       </c>
@@ -6813,7 +6807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>263</v>
       </c>
@@ -6866,7 +6860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>232</v>
       </c>
@@ -6919,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>850</v>
       </c>
@@ -6972,7 +6966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>31</v>
       </c>
@@ -7025,7 +7019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>531</v>
       </c>
@@ -7078,7 +7072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>527</v>
       </c>
@@ -7131,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>600</v>
       </c>
@@ -7184,7 +7178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>549</v>
       </c>
@@ -7237,7 +7231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>338</v>
       </c>
@@ -7287,7 +7281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>717</v>
       </c>
@@ -7340,7 +7334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>809</v>
       </c>
@@ -7390,7 +7384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>755</v>
       </c>
@@ -7443,7 +7437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>620</v>
       </c>
@@ -7496,7 +7490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>767</v>
       </c>
@@ -7546,7 +7540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>828</v>
       </c>
@@ -7596,7 +7590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>134</v>
       </c>
@@ -7649,7 +7643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>351</v>
       </c>
@@ -7702,7 +7696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>693</v>
       </c>
@@ -7755,7 +7749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>362</v>
       </c>
@@ -7805,7 +7799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>561</v>
       </c>
@@ -7858,7 +7852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>509</v>
       </c>
@@ -7911,7 +7905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>821</v>
       </c>
@@ -7961,7 +7955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>777</v>
       </c>
@@ -8011,7 +8005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>731</v>
       </c>
@@ -8064,7 +8058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>786</v>
       </c>
@@ -8114,7 +8108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>714</v>
       </c>
@@ -8167,7 +8161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>772</v>
       </c>
@@ -8220,7 +8214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>448</v>
       </c>
@@ -8273,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>819</v>
       </c>
@@ -8323,7 +8317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>798</v>
       </c>
@@ -8373,7 +8367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>37</v>
       </c>
@@ -8426,7 +8420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>34</v>
       </c>
@@ -8479,7 +8473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>119</v>
       </c>
@@ -8532,7 +8526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>25</v>
       </c>
@@ -8585,7 +8579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>58</v>
       </c>
@@ -8638,7 +8632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>259</v>
       </c>
@@ -8691,7 +8685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>921</v>
       </c>
@@ -8741,7 +8735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>311</v>
       </c>
@@ -8794,7 +8788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>570</v>
       </c>
@@ -8847,7 +8841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>514</v>
       </c>
@@ -8900,7 +8894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>197</v>
       </c>
@@ -8953,7 +8947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>197</v>
       </c>
@@ -9006,7 +9000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>563</v>
       </c>
@@ -9059,7 +9053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>836</v>
       </c>
@@ -9109,7 +9103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>496</v>
       </c>
@@ -9159,7 +9153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>384</v>
       </c>
@@ -9212,7 +9206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>830</v>
       </c>
@@ -9262,7 +9256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>801</v>
       </c>
@@ -9312,7 +9306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>165</v>
       </c>
@@ -9365,7 +9359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>188</v>
       </c>
@@ -9415,7 +9409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>421</v>
       </c>
@@ -9468,7 +9462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>834</v>
       </c>
@@ -9518,7 +9512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>762</v>
       </c>
@@ -9571,7 +9565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>498</v>
       </c>
@@ -9624,7 +9618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>602</v>
       </c>
@@ -9677,7 +9671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>540</v>
       </c>
@@ -9730,7 +9724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>507</v>
       </c>
@@ -9783,7 +9777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>502</v>
       </c>
@@ -9836,7 +9830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>355</v>
       </c>
@@ -9889,7 +9883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>880</v>
       </c>
@@ -9942,7 +9936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>444</v>
       </c>
@@ -9995,7 +9989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>183</v>
       </c>
@@ -10045,7 +10039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>200</v>
       </c>
@@ -10095,7 +10089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>183</v>
       </c>
@@ -10145,7 +10139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>183</v>
       </c>
@@ -10195,7 +10189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>191</v>
       </c>
@@ -10248,7 +10242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>760</v>
       </c>
@@ -10301,7 +10295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>696</v>
       </c>
@@ -10354,7 +10348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>213</v>
       </c>
@@ -10404,7 +10398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>202</v>
       </c>
@@ -10454,7 +10448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>704</v>
       </c>
@@ -10507,7 +10501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>685</v>
       </c>
@@ -10560,7 +10554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>690</v>
       </c>
@@ -10613,7 +10607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>682</v>
       </c>
@@ -10663,7 +10657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>224</v>
       </c>
@@ -10716,7 +10710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>406</v>
       </c>
@@ -10769,7 +10763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>429</v>
       </c>
@@ -10822,7 +10816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>492</v>
       </c>
@@ -10872,7 +10866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>518</v>
       </c>
@@ -10925,7 +10919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>581</v>
       </c>
@@ -10978,7 +10972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>436</v>
       </c>
@@ -11031,7 +11025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>450</v>
       </c>
@@ -11084,7 +11078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>432</v>
       </c>
@@ -11137,7 +11131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>415</v>
       </c>
@@ -11190,7 +11184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>487</v>
       </c>
@@ -11240,7 +11234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>392</v>
       </c>
@@ -11293,7 +11287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>494</v>
       </c>
@@ -11343,7 +11337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>399</v>
       </c>
@@ -11396,7 +11390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>402</v>
       </c>
@@ -11449,7 +11443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>419</v>
       </c>
@@ -11502,7 +11496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>440</v>
       </c>
@@ -11555,7 +11549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>389</v>
       </c>
@@ -11608,7 +11602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>376</v>
       </c>
@@ -11661,7 +11655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>434</v>
       </c>
@@ -11714,7 +11708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>409</v>
       </c>
@@ -11767,7 +11761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>735</v>
       </c>
@@ -11820,7 +11814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>618</v>
       </c>
@@ -11873,7 +11867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>588</v>
       </c>
@@ -11926,7 +11920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>556</v>
       </c>
@@ -11979,7 +11973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>537</v>
       </c>
@@ -12032,7 +12026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>529</v>
       </c>
@@ -12085,7 +12079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>511</v>
       </c>
@@ -12138,7 +12132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>897</v>
       </c>
@@ -12191,7 +12185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>877</v>
       </c>
@@ -12244,7 +12238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>885</v>
       </c>
@@ -12297,7 +12291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>51</v>
       </c>
@@ -12350,7 +12344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>230</v>
       </c>
@@ -12403,7 +12397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>39</v>
       </c>
@@ -12456,7 +12450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>81</v>
       </c>
@@ -12509,7 +12503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>283</v>
       </c>
@@ -12562,7 +12556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>151</v>
       </c>
@@ -12615,7 +12609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>583</v>
       </c>
@@ -12668,7 +12662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>89</v>
       </c>
@@ -12721,7 +12715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>16</v>
       </c>
@@ -12774,7 +12768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>104</v>
       </c>
@@ -12827,7 +12821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>323</v>
       </c>
@@ -12880,7 +12874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>318</v>
       </c>
@@ -12933,7 +12927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>122</v>
       </c>
@@ -12986,7 +12980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>294</v>
       </c>
@@ -13039,7 +13033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>54</v>
       </c>
@@ -13092,7 +13086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>276</v>
       </c>
@@ -13145,7 +13139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>278</v>
       </c>
@@ -13198,7 +13192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>234</v>
       </c>
@@ -13251,7 +13245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>302</v>
       </c>
@@ -13304,7 +13298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>72</v>
       </c>
@@ -13357,7 +13351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>70</v>
       </c>
@@ -13410,7 +13404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>265</v>
       </c>
@@ -13463,7 +13457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>242</v>
       </c>
@@ -13516,7 +13510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>244</v>
       </c>
@@ -13569,7 +13563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>931</v>
       </c>
@@ -13622,7 +13616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>92</v>
       </c>
@@ -13675,7 +13669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>87</v>
       </c>
@@ -13728,7 +13722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>750</v>
       </c>
@@ -13781,7 +13775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>780</v>
       </c>
@@ -13831,7 +13825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>794</v>
       </c>
@@ -13881,7 +13875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>458</v>
       </c>
@@ -13934,7 +13928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>568</v>
       </c>
@@ -13987,7 +13981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>606</v>
       </c>
@@ -14040,7 +14034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>598</v>
       </c>
@@ -14093,7 +14087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>524</v>
       </c>
@@ -14146,7 +14140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>454</v>
       </c>
@@ -14199,7 +14193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>642</v>
       </c>
@@ -14252,7 +14246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>574</v>
       </c>
@@ -14305,7 +14299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>594</v>
       </c>
@@ -14358,7 +14352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>545</v>
       </c>
@@ -14411,7 +14405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>668</v>
       </c>
@@ -14461,7 +14455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>823</v>
       </c>
@@ -14511,7 +14505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>708</v>
       </c>
@@ -14564,7 +14558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>481</v>
       </c>
@@ -14617,7 +14611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>633</v>
       </c>
@@ -14667,7 +14661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>724</v>
       </c>
@@ -14720,7 +14714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>590</v>
       </c>
@@ -14770,7 +14764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>604</v>
       </c>
@@ -14823,7 +14817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>296</v>
       </c>
@@ -14876,7 +14870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>246</v>
       </c>
@@ -14929,7 +14923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>239</v>
       </c>
@@ -14982,7 +14976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>467</v>
       </c>
@@ -15035,7 +15029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>774</v>
       </c>
@@ -15088,7 +15082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>811</v>
       </c>
@@ -15138,7 +15132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>748</v>
       </c>
@@ -15191,7 +15185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>721</v>
       </c>
@@ -15244,7 +15238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>452</v>
       </c>
@@ -15297,7 +15291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>839</v>
       </c>
@@ -15350,7 +15344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>854</v>
       </c>
@@ -15403,7 +15397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>868</v>
       </c>
@@ -15456,7 +15450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>883</v>
       </c>
@@ -15509,7 +15503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>839</v>
       </c>
@@ -15562,7 +15556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>866</v>
       </c>
@@ -15615,7 +15609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>871</v>
       </c>
@@ -15668,7 +15662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>844</v>
       </c>
@@ -15721,7 +15715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>873</v>
       </c>
@@ -15774,7 +15768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>469</v>
       </c>
@@ -15827,7 +15821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>426</v>
       </c>
@@ -15880,7 +15874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>252</v>
       </c>
@@ -15933,7 +15927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>397</v>
       </c>
@@ -15986,7 +15980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>404</v>
       </c>
@@ -16039,7 +16033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>417</v>
       </c>
@@ -16092,7 +16086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>489</v>
       </c>
@@ -16142,7 +16136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>382</v>
       </c>
@@ -16195,7 +16189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>387</v>
       </c>
@@ -16248,7 +16242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>395</v>
       </c>
@@ -16301,7 +16295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>411</v>
       </c>
@@ -16354,7 +16348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>413</v>
       </c>
@@ -16407,7 +16401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>442</v>
       </c>
@@ -16460,7 +16454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>446</v>
       </c>
@@ -16513,7 +16507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>905</v>
       </c>
@@ -16566,7 +16560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>917</v>
       </c>
@@ -16619,7 +16613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>861</v>
       </c>
@@ -16672,7 +16666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>438</v>
       </c>
@@ -16725,7 +16719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>907</v>
       </c>
@@ -16775,7 +16769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>342</v>
       </c>
@@ -16828,7 +16822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>367</v>
       </c>
@@ -16878,7 +16872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>137</v>
       </c>
@@ -16931,7 +16925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>130</v>
       </c>
@@ -16984,7 +16978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>96</v>
       </c>
@@ -17037,7 +17031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>84</v>
       </c>
@@ -17090,7 +17084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>112</v>
       </c>
@@ -17143,7 +17137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>61</v>
       </c>
@@ -17193,7 +17187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>925</v>
       </c>
@@ -17243,7 +17237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>209</v>
       </c>
@@ -17296,7 +17290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>219</v>
       </c>
@@ -17346,7 +17340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>222</v>
       </c>
@@ -17396,7 +17390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>215</v>
       </c>
@@ -17446,7 +17440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>336</v>
       </c>
@@ -17499,7 +17493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>281</v>
       </c>
@@ -17552,7 +17546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>345</v>
       </c>
@@ -17605,7 +17599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>333</v>
       </c>
@@ -17658,7 +17652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>309</v>
       </c>
@@ -17711,7 +17705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>316</v>
       </c>
@@ -17764,7 +17758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>321</v>
       </c>
@@ -17817,7 +17811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>304</v>
       </c>
@@ -17870,7 +17864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>331</v>
       </c>
@@ -17923,7 +17917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>267</v>
       </c>
@@ -17976,7 +17970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>290</v>
       </c>
@@ -18029,7 +18023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
         <v>248</v>
       </c>
@@ -18082,7 +18076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>825</v>
       </c>
@@ -18132,7 +18126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>933</v>
       </c>
@@ -18182,7 +18176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>875</v>
       </c>
@@ -18235,7 +18229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>901</v>
       </c>
@@ -18285,7 +18279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>899</v>
       </c>
@@ -18338,7 +18332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>864</v>
       </c>
@@ -18391,7 +18385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>903</v>
       </c>
@@ -18441,7 +18435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>846</v>
       </c>
@@ -18494,7 +18488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>857</v>
       </c>
@@ -18547,7 +18541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>535</v>
       </c>
@@ -18600,7 +18594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>520</v>
       </c>
@@ -18653,7 +18647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>328</v>
       </c>
@@ -18706,7 +18700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>287</v>
       </c>
@@ -18759,7 +18753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>292</v>
       </c>
@@ -18812,7 +18806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>314</v>
       </c>
@@ -18865,7 +18859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>269</v>
       </c>
@@ -18918,7 +18912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>892</v>
       </c>
@@ -18971,7 +18965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>758</v>
       </c>
@@ -19024,7 +19018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>608</v>
       </c>
@@ -19077,7 +19071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
         <v>577</v>
       </c>
@@ -19130,7 +19124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>596</v>
       </c>
@@ -19183,7 +19177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
         <v>615</v>
       </c>
@@ -19236,7 +19230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>664</v>
       </c>
@@ -19289,7 +19283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>625</v>
       </c>
@@ -19342,7 +19336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>646</v>
       </c>
@@ -19395,7 +19389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>662</v>
       </c>
@@ -19448,7 +19442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>660</v>
       </c>
@@ -19501,7 +19495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>638</v>
       </c>
@@ -19554,7 +19548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>655</v>
       </c>
@@ -19607,7 +19601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>636</v>
       </c>
@@ -19660,7 +19654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
         <v>752</v>
       </c>
@@ -19713,7 +19707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
         <v>648</v>
       </c>
@@ -19766,7 +19760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
         <v>666</v>
       </c>
@@ -19816,7 +19810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
         <v>737</v>
       </c>
@@ -19869,7 +19863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>699</v>
       </c>
@@ -19922,7 +19916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>805</v>
       </c>
@@ -19972,7 +19966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
         <v>792</v>
       </c>
@@ -20022,7 +20016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
         <v>712</v>
       </c>
@@ -20075,7 +20069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
         <v>706</v>
       </c>
@@ -20128,7 +20122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
         <v>733</v>
       </c>
@@ -20181,7 +20175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
         <v>912</v>
       </c>
@@ -20234,7 +20228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>928</v>
       </c>
@@ -20284,7 +20278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
         <v>132</v>
       </c>
@@ -20337,7 +20331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
         <v>114</v>
       </c>
@@ -20390,7 +20384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
         <v>106</v>
       </c>
@@ -20443,7 +20437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
         <v>74</v>
       </c>
@@ -20496,7 +20490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
         <v>153</v>
       </c>
@@ -20546,7 +20540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
         <v>770</v>
       </c>
@@ -20599,7 +20593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>743</v>
       </c>
@@ -20652,7 +20646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
         <v>357</v>
       </c>
@@ -20702,7 +20696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
         <v>365</v>
       </c>
@@ -20752,7 +20746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
         <v>44</v>
       </c>
@@ -20805,7 +20799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>788</v>
       </c>
@@ -20855,7 +20849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
         <v>472</v>
       </c>
@@ -20908,7 +20902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
         <v>485</v>
       </c>
@@ -20961,674 +20955,674 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>